<commit_message>
Code updated for read all sheets from testData.excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/Config/Config.xlsx
+++ b/src/main/resources/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SureshChirra\Desktop\IBM_Projects\Selenium_WS\in.ibm.chirra.saf\src\main\resources\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5FCA5-7804-4C51-B436-A37F4B145C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088F8C0-B2B4-4FDC-96C5-7BD5B5C18D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>7</v>
@@ -637,7 +637,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="2" t="s">

</xml_diff>

<commit_message>
Working project commit 1.
</commit_message>
<xml_diff>
--- a/src/main/resources/Config/Config.xlsx
+++ b/src/main/resources/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SureshChirra\Desktop\IBM_Projects\Selenium_WS\in.ibm.chirra.saf\src\main\resources\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1720F1DE-6506-41C2-B7E7-89E1FE446879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF26257-265E-4CF1-89A4-E1F22FE05A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="2" t="s">

</xml_diff>

<commit_message>
Packages renamed and project commit
</commit_message>
<xml_diff>
--- a/src/main/resources/Config/Config.xlsx
+++ b/src/main/resources/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SureshChirra\Desktop\IBM_Projects\Selenium_WS\in.ibm.chirra.saf\src\main\resources\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF26257-265E-4CF1-89A4-E1F22FE05A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE31B1-4079-498E-A4CC-3BC46C528AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
     <t>Want_To_Rerun_FailedCases_Once</t>
   </si>
   <si>
-    <t>0</t>
+    <t>30</t>
   </si>
 </sst>
 </file>

</xml_diff>